<commit_message>
update file of CR sheet
update file of CR sheet
</commit_message>
<xml_diff>
--- a/Foodies_Sys_Project_Plan/CR_sheet_V1.0.xlsx
+++ b/Foodies_Sys_Project_Plan/CR_sheet_V1.0.xlsx
@@ -7,53 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CR" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
-  </si>
-  <si>
-    <t>Column8</t>
-  </si>
-  <si>
-    <t>Column9</t>
-  </si>
-  <si>
-    <t>Column10</t>
-  </si>
-  <si>
-    <t>Column11</t>
-  </si>
-  <si>
-    <t>Column12</t>
-  </si>
-  <si>
-    <t>Column13</t>
-  </si>
-  <si>
-    <t>Column14</t>
-  </si>
-  <si>
-    <t>Column15</t>
-  </si>
-  <si>
-    <t>Column16</t>
-  </si>
-  <si>
-    <t>Column17</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -65,16 +26,57 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Originator</t>
+  </si>
+  <si>
+    <t>Modifer</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Verifier</t>
+  </si>
+  <si>
+    <t>Date Submitted</t>
+  </si>
+  <si>
+    <t>Date Updated</t>
+  </si>
+  <si>
+    <t>Estimated Hours</t>
+  </si>
+  <si>
+    <t>Change Request</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,8 +102,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -120,28 +128,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:Q2"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:N5" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A4:N5"/>
+  <tableColumns count="14">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Type"/>
     <tableColumn id="3" name="Product Name"/>
+    <tableColumn id="18" name="Title"/>
     <tableColumn id="4" name="Description"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
-    <tableColumn id="9" name="Column9"/>
-    <tableColumn id="10" name="Column10"/>
-    <tableColumn id="11" name="Column11"/>
-    <tableColumn id="12" name="Column12"/>
-    <tableColumn id="13" name="Column13"/>
-    <tableColumn id="14" name="Column14"/>
-    <tableColumn id="15" name="Column15"/>
-    <tableColumn id="16" name="Column16"/>
-    <tableColumn id="17" name="Column17"/>
+    <tableColumn id="5" name="Priority"/>
+    <tableColumn id="6" name="Severity"/>
+    <tableColumn id="7" name="Originator"/>
+    <tableColumn id="8" name="Modifer"/>
+    <tableColumn id="19" name="Verifier"/>
+    <tableColumn id="9" name="Status"/>
+    <tableColumn id="10" name="Date Submitted"/>
+    <tableColumn id="11" name="Date Updated"/>
+    <tableColumn id="12" name="Estimated Hours"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -432,76 +437,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="3" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="10" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>